<commit_message>
Parameter issue is fixed, added Iteration level report event
</commit_message>
<xml_diff>
--- a/HidFW/Datatables/Guru99Bank.xlsx
+++ b/HidFW/Datatables/Guru99Bank.xlsx
@@ -796,10 +796,10 @@
     <t>tests.TC_Login_001</t>
   </si>
   <si>
-    <t>strUserName=mngr207603</t>
-  </si>
-  <si>
-    <t>strPassword=jEbysav</t>
+    <t>strUserName=mngr215089</t>
+  </si>
+  <si>
+    <t>strPassword=AvYtAdu</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:IX3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>